<commit_message>
Calibration excel updated. Cannot relibaly get the first two ewoks.
</commit_message>
<xml_diff>
--- a/CALIBRATION.xlsx
+++ b/CALIBRATION.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06805FD2-0FD8-45EB-8E8D-9CF0A2975377}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF42ABE2-FEDD-4923-ACA9-45CFF74582A9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2159,7 +2159,7 @@
   <dimension ref="A1:K501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>